<commit_message>
update the potential feature engineering transformers column
</commit_message>
<xml_diff>
--- a/data_cleaning_and_feature_engineering.xlsx
+++ b/data_cleaning_and_feature_engineering.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="54">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">Transformed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SmartCorrelationSelector</t>
   </si>
   <si>
     <t xml:space="preserve">Numerical Transformation, SmartCorrelationSelector</t>
@@ -347,7 +350,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,6 +392,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1213,7 +1220,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,262 +1245,284 @@
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="13" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="C20" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="13"/>
+      <c r="B22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C23" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C24" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="18" t="s">
+      <c r="B25" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C25" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="18" t="s">
+      <c r="B26" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C26" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C27" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C28" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="18" t="s">
         <v>52</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>